<commit_message>
se calcula presupuesto mensual
</commit_message>
<xml_diff>
--- a/curso finanzas personales/r1_presupuesto_.xlsx
+++ b/curso finanzas personales/r1_presupuesto_.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <r>
       <rPr>
@@ -287,6 +287,33 @@
   </si>
   <si>
     <t xml:space="preserve">  SUBTOTAL</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Agua</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>Propinas</t>
+  </si>
+  <si>
+    <t>comida</t>
+  </si>
+  <si>
+    <t>cigarros</t>
+  </si>
+  <si>
+    <t>Estacionamiento</t>
   </si>
 </sst>
 </file>
@@ -1617,8 +1644,8 @@
   </sheetPr>
   <dimension ref="B1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="B45" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,19 +1853,21 @@
         <v>7</v>
       </c>
       <c r="E17" s="15"/>
-      <c r="F17" s="41" t="e">
+      <c r="F17" s="41">
         <f t="shared" ref="F17:F22" si="0">E17/$E$22</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="41" t="e">
+      <c r="E18" s="15">
+        <v>200</v>
+      </c>
+      <c r="F18" s="41">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1846,19 +1875,21 @@
         <v>9</v>
       </c>
       <c r="E19" s="15"/>
-      <c r="F19" s="41" t="e">
+      <c r="F19" s="41">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="41" t="e">
+      <c r="E20" s="15">
+        <v>300</v>
+      </c>
+      <c r="F20" s="41">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1866,9 +1897,9 @@
         <v>11</v>
       </c>
       <c r="E21" s="17"/>
-      <c r="F21" s="42" t="e">
+      <c r="F21" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1877,11 +1908,11 @@
       </c>
       <c r="E22" s="23">
         <f>SUM(E17:E21)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="47" t="e">
+        <v>500</v>
+      </c>
+      <c r="F22" s="47">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1899,123 +1930,147 @@
       <c r="F24" s="77"/>
     </row>
     <row r="25" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="24"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="43" t="e">
+      <c r="D25" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="15">
+        <v>389</v>
+      </c>
+      <c r="F25" s="43">
         <f t="shared" ref="F25:F40" si="1">E25/$E$22</f>
-        <v>#DIV/0!</v>
+        <v>0.77800000000000002</v>
       </c>
     </row>
     <row r="26" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="24"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="43" t="e">
+      <c r="D26" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="15">
+        <v>200</v>
+      </c>
+      <c r="F26" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="27" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="24"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="43" t="e">
+      <c r="D27" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="15">
+        <v>238</v>
+      </c>
+      <c r="F27" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.47599999999999998</v>
       </c>
     </row>
     <row r="28" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="44" t="e">
+      <c r="D28" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="26">
+        <v>100</v>
+      </c>
+      <c r="F28" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="24"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="43" t="e">
+      <c r="D29" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="15">
+        <v>200</v>
+      </c>
+      <c r="F29" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="30" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="24"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="43" t="e">
+      <c r="D30" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="15">
+        <v>500</v>
+      </c>
+      <c r="F30" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="25"/>
       <c r="E31" s="26"/>
-      <c r="F31" s="44" t="e">
+      <c r="F31" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="24"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="43" t="e">
+      <c r="F32" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="24"/>
       <c r="E33" s="15"/>
-      <c r="F33" s="43" t="e">
+      <c r="F33" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="28"/>
       <c r="E34" s="17"/>
-      <c r="F34" s="45" t="e">
+      <c r="F34" s="45">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="24"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="43" t="e">
+      <c r="F35" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
-      <c r="F36" s="44" t="e">
+      <c r="F36" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="24"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="43" t="e">
+      <c r="F37" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="24"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="43" t="e">
+      <c r="F38" s="43">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="25"/>
       <c r="E39" s="26"/>
-      <c r="F39" s="44" t="e">
+      <c r="F39" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2024,11 +2079,11 @@
       </c>
       <c r="E40" s="30">
         <f>SUM(E25:E35)</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="46" t="e">
+        <v>1627</v>
+      </c>
+      <c r="F40" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>3.254</v>
       </c>
     </row>
     <row r="41" spans="4:6" s="7" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2044,123 +2099,135 @@
       <c r="F42" s="77"/>
     </row>
     <row r="43" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="24"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="43" t="e">
+      <c r="D43" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="31">
+        <v>30</v>
+      </c>
+      <c r="F43" s="43">
         <f t="shared" ref="F43:F59" si="2">E43/$E$22</f>
-        <v>#DIV/0!</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="44" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="24"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="43" t="e">
+      <c r="D44" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="31">
+        <v>40</v>
+      </c>
+      <c r="F44" s="43">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="45" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="27"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="45" t="e">
+      <c r="D45" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="32">
+        <v>40</v>
+      </c>
+      <c r="F45" s="45">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="46" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D46" s="25"/>
       <c r="E46" s="33"/>
-      <c r="F46" s="44" t="e">
+      <c r="F46" s="44">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="24"/>
       <c r="E47" s="31"/>
-      <c r="F47" s="43" t="e">
+      <c r="F47" s="43">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="24"/>
       <c r="E48" s="31"/>
-      <c r="F48" s="43" t="e">
+      <c r="F48" s="43">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="25"/>
       <c r="E49" s="33"/>
-      <c r="F49" s="44" t="e">
+      <c r="F49" s="44">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="24"/>
       <c r="E50" s="31"/>
-      <c r="F50" s="43" t="e">
+      <c r="F50" s="43">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="25"/>
       <c r="E51" s="33"/>
-      <c r="F51" s="44" t="e">
+      <c r="F51" s="44">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="24"/>
       <c r="E52" s="31"/>
-      <c r="F52" s="43" t="e">
+      <c r="F52" s="43">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="25"/>
       <c r="E53" s="33"/>
-      <c r="F53" s="44" t="e">
+      <c r="F53" s="44">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="24"/>
       <c r="E54" s="31"/>
-      <c r="F54" s="43" t="e">
+      <c r="F54" s="43">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="25"/>
       <c r="E55" s="33"/>
-      <c r="F55" s="44" t="e">
+      <c r="F55" s="44">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="24"/>
       <c r="E56" s="31"/>
-      <c r="F56" s="43" t="e">
+      <c r="F56" s="43">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="27"/>
       <c r="E57" s="38"/>
-      <c r="F57" s="43" t="e">
+      <c r="F57" s="43">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2169,11 +2236,11 @@
       </c>
       <c r="E58" s="37">
         <f>SUM(E43:E57)</f>
-        <v>0</v>
-      </c>
-      <c r="F58" s="48" t="e">
+        <v>110</v>
+      </c>
+      <c r="F58" s="48">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="59" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2182,11 +2249,11 @@
       </c>
       <c r="E59" s="34">
         <f>SUM(E40+E58)</f>
-        <v>0</v>
-      </c>
-      <c r="F59" s="48" t="e">
+        <v>1737</v>
+      </c>
+      <c r="F59" s="48">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>3.4740000000000002</v>
       </c>
       <c r="K59" s="8"/>
     </row>
@@ -2210,11 +2277,11 @@
       </c>
       <c r="E62" s="40">
         <f>E22-E59</f>
-        <v>0</v>
-      </c>
-      <c r="F62" s="49" t="e">
+        <v>-1237</v>
+      </c>
+      <c r="F62" s="49">
         <f>E62/$E$22</f>
-        <v>#DIV/0!</v>
+        <v>-2.4740000000000002</v>
       </c>
       <c r="K62" s="8"/>
     </row>
@@ -2244,8 +2311,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="58" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
primer ejeciio leccion 2 ahorro
</commit_message>
<xml_diff>
--- a/curso finanzas personales/r1_presupuesto_.xlsx
+++ b/curso finanzas personales/r1_presupuesto_.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -315,6 +315,24 @@
   <si>
     <t>Estacionamiento</t>
   </si>
+  <si>
+    <t>comida fuera casa</t>
+  </si>
+  <si>
+    <t>Gasolina</t>
+  </si>
+  <si>
+    <t>mantenimiento moto carro</t>
+  </si>
+  <si>
+    <t>imprevistos</t>
+  </si>
+  <si>
+    <t>salud</t>
+  </si>
+  <si>
+    <t>salidas novia</t>
+  </si>
 </sst>
 </file>
 
@@ -325,7 +343,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +476,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -805,7 +831,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -944,6 +970,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1644,8 +1671,8 @@
   </sheetPr>
   <dimension ref="B1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B45" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61:F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,22 +1879,22 @@
       <c r="D17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="15">
+        <v>300</v>
+      </c>
       <c r="F17" s="41">
         <f t="shared" ref="F17:F22" si="0">E17/$E$22</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="15">
-        <v>200</v>
-      </c>
+      <c r="E18" s="15"/>
       <c r="F18" s="41">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1889,7 +1916,7 @@
       </c>
       <c r="F20" s="41">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1908,7 +1935,7 @@
       </c>
       <c r="E22" s="23">
         <f>SUM(E17:E21)</f>
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="F22" s="47">
         <f t="shared" si="0"/>
@@ -1938,7 +1965,7 @@
       </c>
       <c r="F25" s="43">
         <f t="shared" ref="F25:F40" si="1">E25/$E$22</f>
-        <v>0.77800000000000002</v>
+        <v>0.64833333333333332</v>
       </c>
     </row>
     <row r="26" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1950,7 +1977,7 @@
       </c>
       <c r="F26" s="43">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="27" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1962,7 +1989,7 @@
       </c>
       <c r="F27" s="43">
         <f t="shared" si="1"/>
-        <v>0.47599999999999998</v>
+        <v>0.39666666666666667</v>
       </c>
     </row>
     <row r="28" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1974,7 +2001,7 @@
       </c>
       <c r="F28" s="44">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="29" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1986,7 +2013,7 @@
       </c>
       <c r="F29" s="43">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="30" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1994,19 +2021,23 @@
         <v>27</v>
       </c>
       <c r="E30" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="F30" s="43">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="25"/>
-      <c r="E31" s="26"/>
+      <c r="D31" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="26">
+        <v>300</v>
+      </c>
       <c r="F31" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2079,11 +2110,11 @@
       </c>
       <c r="E40" s="30">
         <f>SUM(E25:E35)</f>
-        <v>1627</v>
+        <v>1727</v>
       </c>
       <c r="F40" s="46">
         <f t="shared" si="1"/>
-        <v>3.254</v>
+        <v>2.8783333333333334</v>
       </c>
     </row>
     <row r="41" spans="4:6" s="7" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2107,7 +2138,7 @@
       </c>
       <c r="F43" s="43">
         <f t="shared" ref="F43:F59" si="2">E43/$E$22</f>
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="44" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2119,7 +2150,7 @@
       </c>
       <c r="F44" s="43">
         <f t="shared" si="2"/>
-        <v>0.08</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="45" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2131,53 +2162,73 @@
       </c>
       <c r="F45" s="45">
         <f t="shared" si="2"/>
-        <v>0.08</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="46" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="25"/>
-      <c r="E46" s="33"/>
+      <c r="D46" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" s="33">
+        <v>200</v>
+      </c>
       <c r="F46" s="44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="47" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="24"/>
-      <c r="E47" s="31"/>
+      <c r="D47" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="31">
+        <v>50</v>
+      </c>
       <c r="F47" s="43">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="48" spans="4:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="24"/>
-      <c r="E48" s="31"/>
+      <c r="D48" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="31">
+        <v>50</v>
+      </c>
       <c r="F48" s="43">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="49" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="25"/>
-      <c r="E49" s="33"/>
+      <c r="D49" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="33">
+        <v>50</v>
+      </c>
       <c r="F49" s="44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="50" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="24"/>
-      <c r="E50" s="31"/>
+      <c r="D50" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="31">
+        <v>100</v>
+      </c>
       <c r="F50" s="43">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="51" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="25"/>
       <c r="E51" s="33"/>
-      <c r="F51" s="44">
+      <c r="F51" s="78">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2236,11 +2287,11 @@
       </c>
       <c r="E58" s="37">
         <f>SUM(E43:E57)</f>
-        <v>110</v>
+        <v>560</v>
       </c>
       <c r="F58" s="48">
         <f t="shared" si="2"/>
-        <v>0.22</v>
+        <v>0.93333333333333335</v>
       </c>
     </row>
     <row r="59" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2249,11 +2300,11 @@
       </c>
       <c r="E59" s="34">
         <f>SUM(E40+E58)</f>
-        <v>1737</v>
+        <v>2287</v>
       </c>
       <c r="F59" s="48">
         <f t="shared" si="2"/>
-        <v>3.4740000000000002</v>
+        <v>3.8116666666666665</v>
       </c>
       <c r="K59" s="8"/>
     </row>
@@ -2277,11 +2328,11 @@
       </c>
       <c r="E62" s="40">
         <f>E22-E59</f>
-        <v>-1237</v>
+        <v>-1687</v>
       </c>
       <c r="F62" s="49">
         <f>E62/$E$22</f>
-        <v>-2.4740000000000002</v>
+        <v>-2.8116666666666665</v>
       </c>
       <c r="K62" s="8"/>
     </row>

</xml_diff>